<commit_message>
Updating some documentation. Adding PCI DSS 3.2 mapping (draft)
</commit_message>
<xml_diff>
--- a/documents/DeploymentTimeline.xlsx
+++ b/documents/DeploymentTimeline.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8184"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8180"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,28 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
-  <si>
-    <t>OMSWorkspaceSolutions</t>
-  </si>
-  <si>
-    <t>DNS Zone</t>
-  </si>
-  <si>
-    <t>Common Infrastructure</t>
-  </si>
-  <si>
-    <t>Application Gateway</t>
-  </si>
-  <si>
-    <t>Bastion Host</t>
-  </si>
-  <si>
-    <t>ASE</t>
-  </si>
-  <si>
-    <t>WebApp and SQL</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
   <si>
     <t>Overall Deploy</t>
   </si>
@@ -65,9 +44,6 @@
     <t>1 min</t>
   </si>
   <si>
-    <t>Automation Account</t>
-  </si>
-  <si>
     <t>2hrs +</t>
   </si>
   <si>
@@ -84,6 +60,36 @@
   </si>
   <si>
     <t>15 mins</t>
+  </si>
+  <si>
+    <t>deploy-OMSWorkspaceSolutions</t>
+  </si>
+  <si>
+    <t>deploy-AutomationAccount</t>
+  </si>
+  <si>
+    <t>deploy-DNSZone</t>
+  </si>
+  <si>
+    <t>deploy-CommonInfrastructure</t>
+  </si>
+  <si>
+    <t>deploy-ApplicationGateway</t>
+  </si>
+  <si>
+    <t>deploy-BastionHostVM</t>
+  </si>
+  <si>
+    <t>deploy-ASE</t>
+  </si>
+  <si>
+    <t>deploy-SQLDB</t>
+  </si>
+  <si>
+    <t>deploy-WebAppAndPackage</t>
+  </si>
+  <si>
+    <t>&lt;2 mins</t>
   </si>
 </sst>
 </file>
@@ -301,12 +307,6 @@
     <xf numFmtId="0" fontId="6" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="2" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
@@ -318,14 +318,24 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="2" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="5" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="7" xfId="5" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="3" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="7" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="7" xfId="6" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="8">
     <cellStyle name="40% - Accent1" xfId="3" builtinId="31"/>
@@ -348,6 +358,392 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>69850</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>209550</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="5" name="Connector: Elbow 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8F8AE56F-D027-41A6-8D39-713E2242CA61}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="16200000" flipH="1">
+          <a:off x="9429750" y="3295650"/>
+          <a:ext cx="311150" cy="209550"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val -1020"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1416050</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="6" name="Connector: Elbow 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CA71DEFF-D612-444F-89F8-F25930CA7BFC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="16200000" flipH="1">
+          <a:off x="3933825" y="2162175"/>
+          <a:ext cx="304800" cy="158750"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="7" name="Connector: Elbow 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E54EFEDA-9F74-4198-97EC-F27C08205C63}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="16200000" flipH="1">
+          <a:off x="3886200" y="2381250"/>
+          <a:ext cx="406400" cy="152400"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>603250</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>146050</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="9" name="Connector: Elbow 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FF082216-0FF3-4013-A493-4FA53EC8823F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="16200000" flipH="1">
+          <a:off x="1946275" y="2625725"/>
+          <a:ext cx="1428750" cy="152400"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 2000"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>603250</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>279400</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="10" name="Connector: Elbow 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{91B45008-687F-420A-903A-AF3390133FC2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="16200000" flipH="1">
+          <a:off x="2098675" y="2466975"/>
+          <a:ext cx="1257300" cy="285750"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val -505"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>711200</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>25400</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="33" name="Connector: Elbow 32">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7161FC2F-E29D-47BF-885B-859A2B9D00CB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="16200000" flipH="1">
+          <a:off x="4594225" y="2867025"/>
+          <a:ext cx="387350" cy="127000"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val -5738"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>12700</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>222250</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="38" name="Connector: Elbow 37">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DB79FBA1-1B07-482E-80F1-6192F4C8A4C8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4838700" y="2717800"/>
+          <a:ext cx="209550" cy="152400"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 50000"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -647,189 +1043,200 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A8:I18"/>
+  <dimension ref="A8:I19"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="I18" sqref="A8:I18"/>
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="21.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.6640625" customWidth="1"/>
-    <col min="5" max="5" width="21.109375" customWidth="1"/>
+    <col min="1" max="1" width="28.36328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.36328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.6328125" customWidth="1"/>
+    <col min="5" max="5" width="21.08984375" customWidth="1"/>
     <col min="7" max="7" width="15" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="21.77734375" customWidth="1"/>
+    <col min="8" max="8" width="21.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="8" spans="1:9" ht="46.8" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:9" ht="47" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="C8" s="20"/>
+      <c r="D8" s="20"/>
+      <c r="E8" s="20"/>
+      <c r="F8" s="20"/>
+      <c r="G8" s="20"/>
+      <c r="H8" s="20"/>
+      <c r="I8" s="20"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A9" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="7"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A10" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" s="10"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="7"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A11" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="11"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="12"/>
+      <c r="E11" s="12"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
+      <c r="I11" s="7"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A12" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="7"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A13" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B13" s="11"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
-      <c r="H8" s="4"/>
-      <c r="I8" s="4"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="6"/>
+      <c r="I13" s="7"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A9" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9" s="7" t="s">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A14" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" s="11"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="F14" s="15"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="6"/>
+      <c r="I14" s="7"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A15" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15" s="11"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="8"/>
-      <c r="H9" s="8"/>
-      <c r="I9" s="9"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="6"/>
+      <c r="I15" s="7"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A10" s="6" t="s">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A16" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B16" s="11"/>
+      <c r="C16" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="D16" s="17"/>
+      <c r="E16" s="17"/>
+      <c r="F16" s="17"/>
+      <c r="G16" s="17"/>
+      <c r="H16" s="17"/>
+      <c r="I16" s="7"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A17" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B17" s="11"/>
+      <c r="C17" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="I17" s="7"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A18" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B18" s="11"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="6"/>
+      <c r="G18" s="6"/>
+      <c r="H18" s="6"/>
+      <c r="I18" s="18" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A19" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B10" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="C10" s="12"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="8"/>
-      <c r="F10" s="8"/>
-      <c r="G10" s="8"/>
-      <c r="H10" s="8"/>
-      <c r="I10" s="9"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A11" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B11" s="13"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="14"/>
-      <c r="E11" s="14"/>
-      <c r="F11" s="8"/>
-      <c r="G11" s="8"/>
-      <c r="H11" s="8"/>
-      <c r="I11" s="9"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A12" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="B12" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="C12" s="8"/>
-      <c r="D12" s="8"/>
-      <c r="E12" s="8"/>
-      <c r="F12" s="8"/>
-      <c r="G12" s="8"/>
-      <c r="H12" s="8"/>
-      <c r="I12" s="9"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A13" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="B13" s="13"/>
-      <c r="C13" s="8"/>
-      <c r="D13" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="E13" s="8"/>
-      <c r="F13" s="8"/>
-      <c r="G13" s="8"/>
-      <c r="H13" s="8"/>
-      <c r="I13" s="9"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A14" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="B14" s="13"/>
-      <c r="C14" s="8"/>
-      <c r="D14" s="8"/>
-      <c r="E14" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="F14" s="18"/>
-      <c r="G14" s="8"/>
-      <c r="H14" s="8"/>
-      <c r="I14" s="9"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A15" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B15" s="13"/>
-      <c r="C15" s="8"/>
-      <c r="D15" s="8"/>
-      <c r="E15" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="F15" s="8"/>
-      <c r="G15" s="8"/>
-      <c r="H15" s="8"/>
-      <c r="I15" s="9"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A16" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B16" s="13"/>
-      <c r="C16" s="20" t="s">
-        <v>10</v>
-      </c>
-      <c r="D16" s="21"/>
-      <c r="E16" s="21"/>
-      <c r="F16" s="21"/>
-      <c r="G16" s="21"/>
-      <c r="H16" s="21"/>
-      <c r="I16" s="9"/>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A17" s="6" t="s">
+      <c r="B19" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="B17" s="13"/>
-      <c r="C17" s="8"/>
-      <c r="D17" s="8"/>
-      <c r="E17" s="8"/>
-      <c r="F17" s="8"/>
-      <c r="G17" s="8"/>
-      <c r="H17" s="8"/>
-      <c r="I17" s="22" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A18" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B18" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
-      <c r="G18" s="1"/>
-      <c r="H18" s="1"/>
-      <c r="I18" s="2"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
+      <c r="I19" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B8:I8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
revised references with recent updates
</commit_message>
<xml_diff>
--- a/documents/DeploymentTimeline.xlsx
+++ b/documents/DeploymentTimeline.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17571"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18201"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pandurangi\Source\Workspaces\Workspace\Samples\ARM-Samples\PCI-PAAS\documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\frasim\Documents\GitHub\pci-paas-webapp-ase-sqldb-appgateway-keyvault-oms\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8180"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8175"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="171027" calcOnSave="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,18 +35,12 @@
     <t>Timeline</t>
   </si>
   <si>
-    <t>2 hrs</t>
-  </si>
-  <si>
     <t>30 secs</t>
   </si>
   <si>
     <t>1 min</t>
   </si>
   <si>
-    <t>2hrs +</t>
-  </si>
-  <si>
     <t>Automated Deployment</t>
   </si>
   <si>
@@ -90,6 +84,12 @@
   </si>
   <si>
     <t>&lt;2 mins</t>
+  </si>
+  <si>
+    <t>1 hrs +</t>
+  </si>
+  <si>
+    <t>1hrs +</t>
   </si>
 </sst>
 </file>
@@ -324,17 +324,17 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="7" xfId="6" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="8">
@@ -364,13 +364,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>15</xdr:row>
       <xdr:rowOff>69850</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>209550</xdr:colOff>
       <xdr:row>17</xdr:row>
       <xdr:rowOff>12700</xdr:rowOff>
@@ -1043,200 +1043,177 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A8:I19"/>
+  <dimension ref="A8:G19"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+      <selection activeCell="O20" sqref="O20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.36328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.36328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.6328125" customWidth="1"/>
-    <col min="5" max="5" width="21.08984375" customWidth="1"/>
-    <col min="7" max="7" width="15" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="21.81640625" customWidth="1"/>
+    <col min="1" max="1" width="28.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5703125" customWidth="1"/>
+    <col min="5" max="5" width="21.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="8" spans="1:9" ht="47" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:7" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="C8" s="20"/>
-      <c r="D8" s="20"/>
-      <c r="E8" s="20"/>
-      <c r="F8" s="20"/>
-      <c r="G8" s="20"/>
-      <c r="H8" s="20"/>
-      <c r="I8" s="20"/>
+      <c r="C8" s="22"/>
+      <c r="D8" s="22"/>
+      <c r="E8" s="22"/>
+      <c r="F8" s="22"/>
+      <c r="G8" s="22"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>1</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C9" s="6"/>
       <c r="D9" s="6"/>
       <c r="E9" s="6"/>
       <c r="F9" s="6"/>
-      <c r="G9" s="6"/>
-      <c r="H9" s="6"/>
-      <c r="I9" s="7"/>
+      <c r="G9" s="7"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C10" s="10"/>
       <c r="D10" s="6"/>
       <c r="E10" s="6"/>
       <c r="F10" s="6"/>
-      <c r="G10" s="6"/>
-      <c r="H10" s="6"/>
-      <c r="I10" s="7"/>
+      <c r="G10" s="7"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B11" s="11"/>
       <c r="C11" s="6"/>
       <c r="D11" s="12"/>
       <c r="E11" s="12"/>
       <c r="F11" s="6"/>
-      <c r="G11" s="6"/>
-      <c r="H11" s="6"/>
-      <c r="I11" s="7"/>
+      <c r="G11" s="7"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B12" s="13" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C12" s="6"/>
       <c r="D12" s="6"/>
       <c r="E12" s="6"/>
       <c r="F12" s="6"/>
-      <c r="G12" s="6"/>
-      <c r="H12" s="6"/>
-      <c r="I12" s="7"/>
+      <c r="G12" s="7"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B13" s="11"/>
       <c r="C13" s="6"/>
       <c r="D13" s="14" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E13" s="6"/>
       <c r="F13" s="6"/>
-      <c r="G13" s="6"/>
-      <c r="H13" s="6"/>
-      <c r="I13" s="7"/>
+      <c r="G13" s="7"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B14" s="11"/>
       <c r="C14" s="6"/>
       <c r="D14" s="6"/>
-      <c r="E14" s="22" t="s">
-        <v>10</v>
+      <c r="E14" s="20" t="s">
+        <v>8</v>
       </c>
       <c r="F14" s="15"/>
-      <c r="G14" s="6"/>
-      <c r="H14" s="6"/>
-      <c r="I14" s="7"/>
+      <c r="G14" s="7"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B15" s="11"/>
       <c r="C15" s="6"/>
       <c r="D15" s="6"/>
-      <c r="E15" s="21" t="s">
-        <v>11</v>
+      <c r="E15" s="19" t="s">
+        <v>9</v>
       </c>
       <c r="F15" s="6"/>
-      <c r="G15" s="6"/>
-      <c r="H15" s="6"/>
-      <c r="I15" s="7"/>
+      <c r="G15" s="7"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B16" s="11"/>
       <c r="C16" s="16" t="s">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="D16" s="17"/>
       <c r="E16" s="17"/>
       <c r="F16" s="17"/>
-      <c r="G16" s="17"/>
-      <c r="H16" s="17"/>
-      <c r="I16" s="7"/>
+      <c r="G16" s="7"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B17" s="11"/>
       <c r="C17" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="I17" s="7"/>
+        <v>19</v>
+      </c>
+      <c r="G17" s="7"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B18" s="11"/>
       <c r="C18" s="6"/>
       <c r="D18" s="6"/>
       <c r="E18" s="6"/>
       <c r="F18" s="6"/>
-      <c r="G18" s="6"/>
-      <c r="H18" s="6"/>
-      <c r="I18" s="18" t="s">
-        <v>5</v>
+      <c r="G18" s="18" t="s">
+        <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
-      <c r="G19" s="1"/>
-      <c r="H19" s="1"/>
-      <c r="I19" s="2"/>
+      <c r="G19" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B8:I8"/>
+    <mergeCell ref="B8:G8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>